<commit_message>
updated results for exp2
</commit_message>
<xml_diff>
--- a/data/EXP 2/exp2_run1_PCR.xlsx
+++ b/data/EXP 2/exp2_run1_PCR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviacattau/Documents/GitHub/fish541_lab/data/EXP 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF97D7E7-B595-F84C-A6C0-27F98CED537A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74558931-D93C-4244-9F99-EE5AC30CEB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32100" yWindow="-1020" windowWidth="27780" windowHeight="17260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32100" yWindow="-1020" windowWidth="27780" windowHeight="17260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cq results" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cq results'!$E$1:$E$97</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -480,9 +480,6 @@
     <t>HSC70</t>
   </si>
   <si>
-    <t>GABB45</t>
-  </si>
-  <si>
     <t>water</t>
   </si>
   <si>
@@ -517,6 +514,9 @@
   </si>
   <si>
     <t>average Cq (HSP70)</t>
+  </si>
+  <si>
+    <t>GADD45</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1045,6 +1045,9 @@
     <xf numFmtId="49" fontId="14" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1362,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5D1C77-129B-D043-927C-FCCCF9546E4E}">
   <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="C50" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58:G92"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -1401,8 +1404,8 @@
       <c r="B2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>146</v>
+      <c r="C2" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>13</v>
@@ -1427,8 +1430,8 @@
       <c r="B3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>146</v>
+      <c r="C3" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>13</v>
@@ -1448,8 +1451,8 @@
       <c r="B4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="30" t="s">
-        <v>146</v>
+      <c r="C4" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>13</v>
@@ -1464,7 +1467,7 @@
         <v>39.08</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -1474,8 +1477,8 @@
       <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="30" t="s">
-        <v>146</v>
+      <c r="C5" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D5" s="30" t="s">
         <v>13</v>
@@ -1493,8 +1496,8 @@
       <c r="B6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="30" t="s">
-        <v>146</v>
+      <c r="C6" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>13</v>
@@ -1519,8 +1522,8 @@
       <c r="B7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>146</v>
+      <c r="C7" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D7" s="30" t="s">
         <v>13</v>
@@ -1540,8 +1543,8 @@
       <c r="B8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>146</v>
+      <c r="C8" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>13</v>
@@ -1566,8 +1569,8 @@
       <c r="B9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="30" t="s">
-        <v>146</v>
+      <c r="C9" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>13</v>
@@ -1587,8 +1590,8 @@
       <c r="B10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>146</v>
+      <c r="C10" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>13</v>
@@ -1606,8 +1609,8 @@
       <c r="B11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="30" t="s">
-        <v>146</v>
+      <c r="C11" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>13</v>
@@ -1625,8 +1628,8 @@
       <c r="B12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>146</v>
+      <c r="C12" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>13</v>
@@ -1651,8 +1654,8 @@
       <c r="B13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="30" t="s">
-        <v>146</v>
+      <c r="C13" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D13" s="30" t="s">
         <v>13</v>
@@ -1672,8 +1675,8 @@
       <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>146</v>
+      <c r="C14" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>13</v>
@@ -1698,8 +1701,8 @@
       <c r="B15" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>146</v>
+      <c r="C15" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D15" s="30" t="s">
         <v>13</v>
@@ -1719,8 +1722,8 @@
       <c r="B16" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="30" t="s">
-        <v>146</v>
+      <c r="C16" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>13</v>
@@ -1745,8 +1748,8 @@
       <c r="B17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="30" t="s">
-        <v>146</v>
+      <c r="C17" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D17" s="30" t="s">
         <v>13</v>
@@ -1766,8 +1769,8 @@
       <c r="B18" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>146</v>
+      <c r="C18" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>13</v>
@@ -1792,8 +1795,8 @@
       <c r="B19" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="30" t="s">
-        <v>146</v>
+      <c r="C19" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D19" s="30" t="s">
         <v>13</v>
@@ -1813,8 +1816,8 @@
       <c r="B20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>146</v>
+      <c r="C20" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>13</v>
@@ -1832,8 +1835,8 @@
       <c r="B21" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="30" t="s">
-        <v>146</v>
+      <c r="C21" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D21" s="30" t="s">
         <v>13</v>
@@ -1851,8 +1854,8 @@
       <c r="B22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="30" t="s">
-        <v>146</v>
+      <c r="C22" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>13</v>
@@ -1870,8 +1873,8 @@
       <c r="B23" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>146</v>
+      <c r="C23" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>13</v>
@@ -1889,8 +1892,8 @@
       <c r="B24" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="30" t="s">
-        <v>146</v>
+      <c r="C24" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>13</v>
@@ -1908,8 +1911,8 @@
       <c r="B25" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>146</v>
+      <c r="C25" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>13</v>
@@ -1927,8 +1930,8 @@
       <c r="B26" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="30" t="s">
-        <v>146</v>
+      <c r="C26" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>13</v>
@@ -1953,8 +1956,8 @@
       <c r="B27" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="30" t="s">
-        <v>146</v>
+      <c r="C27" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>13</v>
@@ -1974,8 +1977,8 @@
       <c r="B28" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>146</v>
+      <c r="C28" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>13</v>
@@ -2000,8 +2003,8 @@
       <c r="B29" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="30" t="s">
-        <v>146</v>
+      <c r="C29" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D29" s="30" t="s">
         <v>13</v>
@@ -2021,8 +2024,8 @@
       <c r="B30" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="30" t="s">
-        <v>146</v>
+      <c r="C30" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>13</v>
@@ -2037,7 +2040,7 @@
         <v>39.6</v>
       </c>
       <c r="H30" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.15">
@@ -2047,8 +2050,8 @@
       <c r="B31" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="30" t="s">
-        <v>146</v>
+      <c r="C31" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D31" s="30" t="s">
         <v>13</v>
@@ -2066,8 +2069,8 @@
       <c r="B32" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="30" t="s">
-        <v>146</v>
+      <c r="C32" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>13</v>
@@ -2085,8 +2088,8 @@
       <c r="B33" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="30" t="s">
-        <v>146</v>
+      <c r="C33" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D33" s="30" t="s">
         <v>13</v>
@@ -2104,8 +2107,8 @@
       <c r="B34" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="30" t="s">
-        <v>146</v>
+      <c r="C34" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>13</v>
@@ -2130,8 +2133,8 @@
       <c r="B35" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="30" t="s">
-        <v>146</v>
+      <c r="C35" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D35" s="30" t="s">
         <v>13</v>
@@ -2151,8 +2154,8 @@
       <c r="B36" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="30" t="s">
-        <v>146</v>
+      <c r="C36" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>13</v>
@@ -2165,7 +2168,7 @@
         <v>38.08</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.15">
@@ -2175,8 +2178,8 @@
       <c r="B37" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="30" t="s">
-        <v>146</v>
+      <c r="C37" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D37" s="30" t="s">
         <v>13</v>
@@ -2196,14 +2199,14 @@
       <c r="B38" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="F38" s="31"/>
       <c r="H38" s="32">
@@ -2217,14 +2220,14 @@
       <c r="B39" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="66" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="34" t="s">
         <v>146</v>
-      </c>
-      <c r="D39" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="34" t="s">
-        <v>147</v>
       </c>
       <c r="F39" s="31"/>
       <c r="H39" s="32"/>
@@ -2236,8 +2239,8 @@
       <c r="B40" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="30" t="s">
-        <v>146</v>
+      <c r="C40" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>13</v>
@@ -2253,8 +2256,8 @@
       <c r="B41" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="30" t="s">
-        <v>146</v>
+      <c r="C41" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D41" s="30" t="s">
         <v>13</v>
@@ -2270,8 +2273,8 @@
       <c r="B42" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C42" s="30" t="s">
-        <v>146</v>
+      <c r="C42" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>13</v>
@@ -2287,8 +2290,8 @@
       <c r="B43" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="30" t="s">
-        <v>146</v>
+      <c r="C43" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D43" s="30" t="s">
         <v>13</v>
@@ -2304,8 +2307,8 @@
       <c r="B44" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="30" t="s">
-        <v>146</v>
+      <c r="C44" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D44" s="30" t="s">
         <v>13</v>
@@ -2321,8 +2324,8 @@
       <c r="B45" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="30" t="s">
-        <v>146</v>
+      <c r="C45" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D45" s="30" t="s">
         <v>13</v>
@@ -2338,8 +2341,8 @@
       <c r="B46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="30" t="s">
-        <v>146</v>
+      <c r="C46" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>13</v>
@@ -2355,8 +2358,8 @@
       <c r="B47" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="30" t="s">
-        <v>146</v>
+      <c r="C47" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D47" s="30" t="s">
         <v>13</v>
@@ -2372,8 +2375,8 @@
       <c r="B48" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="30" t="s">
-        <v>146</v>
+      <c r="C48" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>13</v>
@@ -2389,8 +2392,8 @@
       <c r="B49" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="30" t="s">
-        <v>146</v>
+      <c r="C49" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D49" s="30" t="s">
         <v>13</v>
@@ -2406,8 +2409,8 @@
       <c r="B50" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="30" t="s">
-        <v>146</v>
+      <c r="C50" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D50" s="30" t="s">
         <v>13</v>
@@ -2423,8 +2426,8 @@
       <c r="B51" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="30" t="s">
-        <v>146</v>
+      <c r="C51" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D51" s="30" t="s">
         <v>13</v>
@@ -2440,8 +2443,8 @@
       <c r="B52" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="30" t="s">
-        <v>146</v>
+      <c r="C52" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>13</v>
@@ -2457,8 +2460,8 @@
       <c r="B53" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="30" t="s">
-        <v>146</v>
+      <c r="C53" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D53" s="30" t="s">
         <v>13</v>
@@ -2474,8 +2477,8 @@
       <c r="B54" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="30" t="s">
-        <v>146</v>
+      <c r="C54" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D54" s="30" t="s">
         <v>13</v>
@@ -2491,8 +2494,8 @@
       <c r="B55" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="30" t="s">
-        <v>146</v>
+      <c r="C55" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D55" s="30" t="s">
         <v>13</v>
@@ -2508,8 +2511,8 @@
       <c r="B56" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="30" t="s">
-        <v>146</v>
+      <c r="C56" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>13</v>
@@ -2525,8 +2528,8 @@
       <c r="B57" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="30" t="s">
-        <v>146</v>
+      <c r="C57" s="66" t="s">
+        <v>158</v>
       </c>
       <c r="D57" s="30" t="s">
         <v>13</v>
@@ -3124,7 +3127,7 @@
         <v>27.41</v>
       </c>
       <c r="H82" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.15">
@@ -3416,7 +3419,7 @@
         <v>13</v>
       </c>
       <c r="E95" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F95" s="31"/>
       <c r="G95">
@@ -3473,7 +3476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC933DB-52CD-9A4B-8135-19191370B34C}">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -3493,34 +3496,34 @@
         <v>4</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>158</v>
-      </c>
       <c r="E1" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="G1" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="I1" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="K1" s="59" t="s">
         <v>154</v>
-      </c>
-      <c r="K1" s="59" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="48" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
@@ -4009,13 +4012,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4027,13 +4030,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D21">
         <v>0</v>

</xml_diff>